<commit_message>
added doc, edited maze
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\straw\Desktop\AIS\ProjectPool 1\Maze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2009E13D-5DE6-4242-8ADA-C65A25A88D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFBA34B-383F-43BB-8C98-3BADAFFBA53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Ajouté par</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>comprendre recursive backtracking</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=elMXlO28Q1U&amp;t=265s</t>
+  </si>
+  <si>
+    <t>Maze Generation Algorithm - Recursive Backtracker</t>
   </si>
 </sst>
 </file>
@@ -389,16 +395,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" customWidth="1"/>
     <col min="3" max="3" width="34.7265625" customWidth="1"/>
     <col min="4" max="4" width="84.26953125" customWidth="1"/>
   </cols>
@@ -481,6 +487,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -488,6 +508,7 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{94A60B56-50D9-4655-A1B3-BDC44E9BDC79}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{63E0BEAE-8C89-4ADA-B3D1-7C47A49EAB89}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{D3F2A01D-DAE9-41D5-BD37-47C2A475C72A}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{6935ACF6-CB47-481E-8259-A04464879C35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>